<commit_message>
update checklist of messages
</commit_message>
<xml_diff>
--- a/Supplementary/message-checklist.xlsx
+++ b/Supplementary/message-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\AIS RECEIVER\AISParser\Supplementary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDD9905-D879-4DC0-A7EE-3F7CB97A98BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D464BDE-CE5D-404F-99F9-664DACDA2917}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{43B057C8-1EB0-4194-90C5-3525B64C2E4B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
   <si>
     <t>Message</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Static</t>
+  </si>
+  <si>
+    <t>Clarity is required, flag is not specified</t>
   </si>
 </sst>
 </file>
@@ -130,7 +133,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -140,6 +143,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -156,12 +165,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,16 +486,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85D7DD10-6DE0-4C48-B78D-F863D2250392}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="42.109375" customWidth="1"/>
     <col min="2" max="2" width="12.77734375" customWidth="1"/>
+    <col min="4" max="4" width="32.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -652,7 +663,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -662,8 +673,11 @@
       <c r="C17" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -671,7 +685,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -679,7 +693,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -687,7 +701,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -698,7 +712,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>

</xml_diff>